<commit_message>
[ANV] added a percent of captures column
</commit_message>
<xml_diff>
--- a/levelfiles/spreadsheet/iodine.xlsx
+++ b/levelfiles/spreadsheet/iodine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/villaa/Computing/nrCascadeSim/levelfiles/spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6A1DA4-552E-5445-97B4-F88FFD3BE1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC14688A-CE36-C34B-B853-9C0163248602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="760" windowWidth="28040" windowHeight="17040" xr2:uid="{2D1C8EBD-58BF-0748-ACC6-F1ED1991D975}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>iso</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>Sn (MeV)</t>
+  </si>
+  <si>
+    <t>Cap. Percent (%)</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{269F673A-9A68-9948-B26F-F24DE369A567}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,10 +421,10 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="6" max="7" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +443,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>127</v>
       </c>
@@ -462,11 +468,19 @@
       <c r="F2">
         <v>6.82613</v>
       </c>
+      <c r="G2">
+        <f>(D2/$D$3)*100</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3">
         <f>SUM(C2:C2)</f>
         <v>100</v>
+      </c>
+      <c r="D3">
+        <f>SUM(D2:D2)</f>
+        <v>640.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>